<commit_message>
update no processo ecxel
</commit_message>
<xml_diff>
--- a/processo.xlsx
+++ b/processo.xlsx
@@ -135,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,12 +174,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -210,13 +204,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +494,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,18 +506,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -567,7 +561,7 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -582,18 +576,18 @@
       <c r="C10" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -663,18 +657,18 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -724,7 +718,8 @@
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="10"/>
+      <c r="D32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
fix na quantidade de impressões
</commit_message>
<xml_diff>
--- a/processo.xlsx
+++ b/processo.xlsx
@@ -204,13 +204,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,18 +506,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -576,18 +576,18 @@
       <c r="C10" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -657,18 +657,18 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -706,7 +706,8 @@
       <c r="A30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -718,7 +719,7 @@
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="10"/>
+      <c r="B32" s="8"/>
       <c r="D32" s="3"/>
     </row>
   </sheetData>

</xml_diff>